<commit_message>
typo in data, corrected now
</commit_message>
<xml_diff>
--- a/Data/Arran_GBIF_Data.xlsx
+++ b/Data/Arran_GBIF_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jojosunderland/Documents/WorkingD/EcIA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC476C1-7B13-8B41-B649-AA701BC699A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA0E3F5-31C9-6844-97E5-22C9CC235DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="760" windowWidth="26300" windowHeight="16660" activeTab="7" xr2:uid="{372C8A34-AC94-F84B-AFF8-3FA7D794AB3F}"/>
   </bookViews>
@@ -47961,8 +47961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725C5465-E8B2-9A43-988E-5F8B7BFB7015}">
   <dimension ref="A1:AE303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="F306" sqref="F306"/>
+    <sheetView tabSelected="1" topLeftCell="R275" workbookViewId="0">
+      <selection activeCell="AB101" sqref="AB101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -56786,7 +56786,7 @@
         <v>48</v>
       </c>
       <c r="AB95" s="4" t="s">
-        <v>239</v>
+        <v>49</v>
       </c>
       <c r="AC95" s="4" t="s">
         <v>221</v>

</xml_diff>